<commit_message>
updating for the new quarter -- fixed a broken link
</commit_message>
<xml_diff>
--- a/modules/data/Sauk_peak_WY1929_2017.xlsx
+++ b/modules/data/Sauk_peak_WY1929_2017.xlsx
@@ -1,16 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10711"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdlund/Documents/CEE465_GitHubclone/data-analysis/modules/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B1E749-D707-BA42-9003-236AFF1A9898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47440" yWindow="1660" windowWidth="25600" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sauk_peak_1928_2017.txt" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -63,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -102,6 +117,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -426,46 +449,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -479,7 +502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -493,7 +516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1929</v>
       </c>
@@ -507,7 +530,7 @@
         <v>9.33</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <f>A9+1</f>
         <v>1930</v>
@@ -522,7 +545,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ref="A11:A74" si="0">A10+1</f>
         <v>1931</v>
@@ -537,7 +560,7 @@
         <v>9.32</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1932</v>
@@ -552,7 +575,7 @@
         <v>15.83</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1933</v>
@@ -567,7 +590,7 @@
         <v>12.62</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>1934</v>
@@ -582,7 +605,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>1935</v>
@@ -597,7 +620,7 @@
         <v>13.54</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>1936</v>
@@ -612,7 +635,7 @@
         <v>8.33</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>1937</v>
@@ -627,7 +650,7 @@
         <v>8.15</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>1938</v>
@@ -642,7 +665,7 @@
         <v>10.78</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>1939</v>
@@ -657,7 +680,7 @@
         <v>9.9600000000000009</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>1940</v>
@@ -672,7 +695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>1941</v>
@@ -687,7 +710,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>1942</v>
@@ -702,7 +725,7 @@
         <v>8.85</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>1943</v>
@@ -717,7 +740,7 @@
         <v>9.02</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>1944</v>
@@ -732,7 +755,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>1945</v>
@@ -747,7 +770,7 @@
         <v>10.28</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>1946</v>
@@ -762,7 +785,7 @@
         <v>9.9600000000000009</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>1947</v>
@@ -777,7 +800,7 @@
         <v>11.41</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>1948</v>
@@ -792,7 +815,7 @@
         <v>11.74</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>1949</v>
@@ -807,7 +830,7 @@
         <v>9.0299999999999994</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>1950</v>
@@ -822,7 +845,7 @@
         <v>16.93</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>1951</v>
@@ -837,7 +860,7 @@
         <v>14.97</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>1952</v>
@@ -852,7 +875,7 @@
         <v>7.65</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>1953</v>
@@ -867,7 +890,7 @@
         <v>10.56</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>1954</v>
@@ -882,7 +905,7 @@
         <v>8.17</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>1955</v>
@@ -897,7 +920,7 @@
         <v>9.56</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>1956</v>
@@ -912,7 +935,7 @@
         <v>12.23</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>1957</v>
@@ -927,7 +950,7 @@
         <v>10.41</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>1958</v>
@@ -942,7 +965,7 @@
         <v>7.94</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>1959</v>
@@ -957,7 +980,7 @@
         <v>11.59</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>1960</v>
@@ -972,7 +995,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>1961</v>
@@ -987,7 +1010,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>1962</v>
@@ -1002,7 +1025,7 @@
         <v>10.27</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>1963</v>
@@ -1017,7 +1040,7 @@
         <v>12.83</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>1964</v>
@@ -1032,7 +1055,7 @@
         <v>9.65</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>1965</v>
@@ -1047,7 +1070,7 @@
         <v>9.73</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>1966</v>
@@ -1062,7 +1085,7 @@
         <v>8.23</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>1967</v>
@@ -1077,7 +1100,7 @@
         <v>10.26</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>1968</v>
@@ -1092,7 +1115,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>1969</v>
@@ -1107,7 +1130,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>1970</v>
@@ -1122,7 +1145,7 @@
         <v>8.52</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>1971</v>
@@ -1137,7 +1160,7 @@
         <v>10.98</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>1972</v>
@@ -1152,7 +1175,7 @@
         <v>10.92</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>1973</v>
@@ -1167,7 +1190,7 @@
         <v>10.09</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>1974</v>
@@ -1182,7 +1205,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>1975</v>
@@ -1197,7 +1220,7 @@
         <v>11.61</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>1976</v>
@@ -1212,7 +1235,7 @@
         <v>15.03</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>1977</v>
@@ -1227,7 +1250,7 @@
         <v>10.42</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>1978</v>
@@ -1242,7 +1265,7 @@
         <v>11.55</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>1979</v>
@@ -1257,7 +1280,7 @@
         <v>9.3800000000000008</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>1980</v>
@@ -1272,7 +1295,7 @@
         <v>14.27</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>1981</v>
@@ -1287,7 +1310,7 @@
         <v>18.239999999999998</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>1982</v>
@@ -1302,7 +1325,7 @@
         <v>10.26</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>1983</v>
@@ -1317,7 +1340,7 @@
         <v>13.84</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>1984</v>
@@ -1332,7 +1355,7 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>1985</v>
@@ -1347,7 +1370,7 @@
         <v>9.4600000000000009</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>1986</v>
@@ -1362,7 +1385,7 @@
         <v>13.22</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>1987</v>
@@ -1377,7 +1400,7 @@
         <v>12.44</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
         <f t="shared" si="0"/>
         <v>1988</v>
@@ -1392,7 +1415,7 @@
         <v>8.8800000000000008</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
         <f t="shared" si="0"/>
         <v>1989</v>
@@ -1407,7 +1430,7 @@
         <v>11.54</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
         <f t="shared" si="0"/>
         <v>1990</v>
@@ -1422,7 +1445,7 @@
         <v>14.55</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
         <f t="shared" si="0"/>
         <v>1991</v>
@@ -1437,7 +1460,7 @@
         <v>16.989999999999998</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
         <f t="shared" si="0"/>
         <v>1992</v>
@@ -1452,7 +1475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
         <f t="shared" si="0"/>
         <v>1993</v>
@@ -1467,7 +1490,7 @@
         <v>8.5399999999999991</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
         <f t="shared" si="0"/>
         <v>1994</v>
@@ -1482,7 +1505,7 @@
         <v>8.1300000000000008</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
         <f t="shared" ref="A75:A97" si="1">A74+1</f>
         <v>1995</v>
@@ -1497,7 +1520,7 @@
         <v>10.92</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>1996</v>
@@ -1512,7 +1535,7 @@
         <v>16.57</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>1997</v>
@@ -1527,7 +1550,7 @@
         <v>11.75</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>1998</v>
@@ -1542,7 +1565,7 @@
         <v>12.24</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>1999</v>
@@ -1557,7 +1580,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>2000</v>
@@ -1572,7 +1595,7 @@
         <v>13.03</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>2001</v>
@@ -1587,7 +1610,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>2002</v>
@@ -1602,7 +1625,7 @@
         <v>13.32</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>2003</v>
@@ -1617,7 +1640,7 @@
         <v>11.45</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>2004</v>
@@ -1632,7 +1655,7 @@
         <v>18.96</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>2005</v>
@@ -1647,7 +1670,7 @@
         <v>13.84</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>2006</v>
@@ -1662,7 +1685,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>2007</v>
@@ -1677,7 +1700,7 @@
         <v>17.13</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>2008</v>
@@ -1692,7 +1715,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>2009</v>
@@ -1707,7 +1730,7 @@
         <v>12.18</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>2010</v>
@@ -1722,7 +1745,7 @@
         <v>10.130000000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>2011</v>
@@ -1737,7 +1760,7 @@
         <v>13.21</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>2012</v>
@@ -1752,7 +1775,7 @@
         <v>9.48</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>2013</v>
@@ -1767,7 +1790,7 @@
         <v>9.36</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>2014</v>
@@ -1782,7 +1805,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>2015</v>
@@ -1797,7 +1820,7 @@
         <v>12.62</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>2016</v>
@@ -1812,7 +1835,7 @@
         <v>14.28</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>2017</v>
@@ -1825,6 +1848,48 @@
       </c>
       <c r="D97">
         <v>11.63</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>2018</v>
+      </c>
+      <c r="B98" s="1">
+        <v>41600</v>
+      </c>
+      <c r="C98">
+        <v>61900</v>
+      </c>
+      <c r="D98">
+        <v>14.09</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>2019</v>
+      </c>
+      <c r="B99" s="1">
+        <v>41969</v>
+      </c>
+      <c r="C99">
+        <v>27900</v>
+      </c>
+      <c r="D99">
+        <v>9.8699999999999992</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>2020</v>
+      </c>
+      <c r="B100" s="1">
+        <v>42400</v>
+      </c>
+      <c r="C100">
+        <v>50000</v>
+      </c>
+      <c r="D100">
+        <v>12.71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>